<commit_message>
tugas 3 database mysql
</commit_message>
<xml_diff>
--- a/studi kasus.xlsx
+++ b/studi kasus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Documents\Budi Luhur\Semester 6\PT Hendevane Indonesia\Database MySQL\tugas 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D44F225E-0B1D-4886-A068-B9830E323FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25D5CC3-2CD1-45C2-8E70-2FCD587A7B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="2970" windowWidth="21600" windowHeight="11295" xr2:uid="{A3CE01AA-DE0C-4D74-ADEF-BF9CEF8857CC}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{A3CE01AA-DE0C-4D74-ADEF-BF9CEF8857CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="20">
   <si>
     <t>no pengajuan</t>
   </si>
@@ -73,6 +73,18 @@
   </si>
   <si>
     <t>biro administrasi</t>
+  </si>
+  <si>
+    <t>1NF</t>
+  </si>
+  <si>
+    <t>2NF</t>
+  </si>
+  <si>
+    <t>3NF</t>
+  </si>
+  <si>
+    <t>id_satuan_kerja</t>
   </si>
 </sst>
 </file>
@@ -136,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -145,7 +157,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,21 +478,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FA22C68-C8C5-4179-987D-346017962F0B}">
-  <dimension ref="B3:H15"/>
+  <dimension ref="B3:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60:I72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -513,10 +532,10 @@
       <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="6">
         <v>43831</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="6">
         <v>43833</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -530,10 +549,10 @@
       <c r="C5" s="3"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="4">
+      <c r="F5" s="6">
         <v>43845</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="6">
         <v>43847</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -547,10 +566,10 @@
       <c r="C6" s="3"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="4">
+      <c r="F6" s="6">
         <v>43850</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="6">
         <v>43850</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -564,10 +583,10 @@
       <c r="C7" s="3"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="4">
+      <c r="F7" s="6">
         <v>43864</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="6">
         <v>43865</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -581,10 +600,10 @@
       <c r="C8" s="3"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="4">
+      <c r="F8" s="6">
         <v>43898</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="6">
         <v>43900</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -598,10 +617,10 @@
       <c r="C9" s="3"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="4">
+      <c r="F9" s="6">
         <v>43926</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="6">
         <v>43926</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -621,10 +640,10 @@
       <c r="E10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="6">
         <v>43832</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="6">
         <v>43832</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -638,10 +657,10 @@
       <c r="C11" s="3"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="4">
+      <c r="F11" s="6">
         <v>43865</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="6">
         <v>43868</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -655,10 +674,10 @@
       <c r="C12" s="3"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="4">
+      <c r="F12" s="6">
         <v>43895</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="6">
         <v>43900</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -678,10 +697,10 @@
       <c r="E13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="6">
         <v>43925</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="6">
         <v>43926</v>
       </c>
       <c r="H13" s="1" t="s">
@@ -701,10 +720,10 @@
       <c r="E14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="6">
         <v>43878</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="6">
         <v>43880</v>
       </c>
       <c r="H14" s="1" t="s">
@@ -718,13 +737,897 @@
       <c r="C15" s="3"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="4">
+      <c r="F15" s="6">
         <v>43913</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="6">
         <v>43918</v>
       </c>
       <c r="H15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3">
+        <v>10001</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="6">
+        <v>43831</v>
+      </c>
+      <c r="G20" s="6">
+        <v>43833</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>2</v>
+      </c>
+      <c r="C21" s="3">
+        <v>10001</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="6">
+        <v>43845</v>
+      </c>
+      <c r="G21" s="6">
+        <v>43847</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>3</v>
+      </c>
+      <c r="C22" s="3">
+        <v>10001</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="6">
+        <v>43850</v>
+      </c>
+      <c r="G22" s="6">
+        <v>43850</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>4</v>
+      </c>
+      <c r="C23" s="3">
+        <v>10001</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="6">
+        <v>43864</v>
+      </c>
+      <c r="G23" s="6">
+        <v>43865</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>5</v>
+      </c>
+      <c r="C24" s="3">
+        <v>10001</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="6">
+        <v>43898</v>
+      </c>
+      <c r="G24" s="6">
+        <v>43900</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>6</v>
+      </c>
+      <c r="C25" s="3">
+        <v>10001</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="6">
+        <v>43926</v>
+      </c>
+      <c r="G25" s="6">
+        <v>43926</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>7</v>
+      </c>
+      <c r="C26" s="3">
+        <v>10032</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="6">
+        <v>43832</v>
+      </c>
+      <c r="G26" s="6">
+        <v>43832</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>8</v>
+      </c>
+      <c r="C27" s="3">
+        <v>10032</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="6">
+        <v>43865</v>
+      </c>
+      <c r="G27" s="6">
+        <v>43868</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <v>9</v>
+      </c>
+      <c r="C28" s="3">
+        <v>10032</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="6">
+        <v>43895</v>
+      </c>
+      <c r="G28" s="6">
+        <v>43900</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <v>10</v>
+      </c>
+      <c r="C29" s="3">
+        <v>10044</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="6">
+        <v>43925</v>
+      </c>
+      <c r="G29" s="6">
+        <v>43926</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>11</v>
+      </c>
+      <c r="C30" s="3">
+        <v>10021</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="6">
+        <v>43878</v>
+      </c>
+      <c r="G30" s="6">
+        <v>43880</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>12</v>
+      </c>
+      <c r="C31" s="3">
+        <v>10021</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="6">
+        <v>43913</v>
+      </c>
+      <c r="G31" s="6">
+        <v>43918</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="1">
+        <v>10001</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1</v>
+      </c>
+      <c r="G38" s="6">
+        <v>43831</v>
+      </c>
+      <c r="H38" s="6">
+        <v>43833</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="1">
+        <v>10032</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39" s="1">
+        <v>2</v>
+      </c>
+      <c r="G39" s="6">
+        <v>43845</v>
+      </c>
+      <c r="H39" s="6">
+        <v>43847</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="1">
+        <v>10044</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="1">
+        <v>3</v>
+      </c>
+      <c r="G40" s="6">
+        <v>43850</v>
+      </c>
+      <c r="H40" s="6">
+        <v>43850</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="1">
+        <v>10021</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" s="1">
+        <v>4</v>
+      </c>
+      <c r="G41" s="6">
+        <v>43864</v>
+      </c>
+      <c r="H41" s="6">
+        <v>43865</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="1">
+        <v>5</v>
+      </c>
+      <c r="G42" s="6">
+        <v>43898</v>
+      </c>
+      <c r="H42" s="6">
+        <v>43900</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F43" s="1">
+        <v>6</v>
+      </c>
+      <c r="G43" s="6">
+        <v>43926</v>
+      </c>
+      <c r="H43" s="6">
+        <v>43926</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F44" s="1">
+        <v>7</v>
+      </c>
+      <c r="G44" s="6">
+        <v>43832</v>
+      </c>
+      <c r="H44" s="6">
+        <v>43832</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F45" s="1">
+        <v>8</v>
+      </c>
+      <c r="G45" s="6">
+        <v>43865</v>
+      </c>
+      <c r="H45" s="6">
+        <v>43868</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F46" s="1">
+        <v>9</v>
+      </c>
+      <c r="G46" s="6">
+        <v>43895</v>
+      </c>
+      <c r="H46" s="6">
+        <v>43900</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F47" s="1">
+        <v>10</v>
+      </c>
+      <c r="G47" s="6">
+        <v>43925</v>
+      </c>
+      <c r="H47" s="6">
+        <v>43926</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F48" s="1">
+        <v>11</v>
+      </c>
+      <c r="G48" s="6">
+        <v>43878</v>
+      </c>
+      <c r="H48" s="6">
+        <v>43880</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F49" s="1">
+        <v>12</v>
+      </c>
+      <c r="G49" s="6">
+        <v>43913</v>
+      </c>
+      <c r="H49" s="6">
+        <v>43918</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="1">
+        <v>10001</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54" s="1">
+        <v>1</v>
+      </c>
+      <c r="F54" s="1">
+        <v>1</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="1">
+        <v>10032</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="1">
+        <v>2</v>
+      </c>
+      <c r="F55" s="1">
+        <v>2</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="1">
+        <v>10044</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="1">
+        <v>1</v>
+      </c>
+      <c r="F56" s="1">
+        <v>3</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B57" s="1">
+        <v>10021</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B60" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B61" s="1">
+        <v>1</v>
+      </c>
+      <c r="C61" s="3">
+        <v>10001</v>
+      </c>
+      <c r="F61" s="1">
+        <v>1</v>
+      </c>
+      <c r="G61" s="6">
+        <v>43831</v>
+      </c>
+      <c r="H61" s="6">
+        <v>43833</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B62" s="1">
+        <v>2</v>
+      </c>
+      <c r="C62" s="3">
+        <v>10001</v>
+      </c>
+      <c r="F62" s="1">
+        <v>2</v>
+      </c>
+      <c r="G62" s="6">
+        <v>43845</v>
+      </c>
+      <c r="H62" s="6">
+        <v>43847</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B63" s="1">
+        <v>3</v>
+      </c>
+      <c r="C63" s="3">
+        <v>10001</v>
+      </c>
+      <c r="F63" s="1">
+        <v>3</v>
+      </c>
+      <c r="G63" s="6">
+        <v>43850</v>
+      </c>
+      <c r="H63" s="6">
+        <v>43850</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B64" s="1">
+        <v>4</v>
+      </c>
+      <c r="C64" s="3">
+        <v>10001</v>
+      </c>
+      <c r="F64" s="1">
+        <v>4</v>
+      </c>
+      <c r="G64" s="6">
+        <v>43864</v>
+      </c>
+      <c r="H64" s="6">
+        <v>43865</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B65" s="1">
+        <v>5</v>
+      </c>
+      <c r="C65" s="3">
+        <v>10001</v>
+      </c>
+      <c r="F65" s="1">
+        <v>5</v>
+      </c>
+      <c r="G65" s="6">
+        <v>43898</v>
+      </c>
+      <c r="H65" s="6">
+        <v>43900</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B66" s="1">
+        <v>6</v>
+      </c>
+      <c r="C66" s="3">
+        <v>10001</v>
+      </c>
+      <c r="F66" s="1">
+        <v>6</v>
+      </c>
+      <c r="G66" s="6">
+        <v>43926</v>
+      </c>
+      <c r="H66" s="6">
+        <v>43926</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B67" s="1">
+        <v>7</v>
+      </c>
+      <c r="C67" s="3">
+        <v>10032</v>
+      </c>
+      <c r="F67" s="1">
+        <v>7</v>
+      </c>
+      <c r="G67" s="6">
+        <v>43832</v>
+      </c>
+      <c r="H67" s="6">
+        <v>43832</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B68" s="1">
+        <v>8</v>
+      </c>
+      <c r="C68" s="3">
+        <v>10032</v>
+      </c>
+      <c r="F68" s="1">
+        <v>8</v>
+      </c>
+      <c r="G68" s="6">
+        <v>43865</v>
+      </c>
+      <c r="H68" s="6">
+        <v>43868</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B69" s="1">
+        <v>9</v>
+      </c>
+      <c r="C69" s="3">
+        <v>10032</v>
+      </c>
+      <c r="F69" s="1">
+        <v>9</v>
+      </c>
+      <c r="G69" s="6">
+        <v>43895</v>
+      </c>
+      <c r="H69" s="6">
+        <v>43900</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B70" s="1">
+        <v>10</v>
+      </c>
+      <c r="C70" s="3">
+        <v>10044</v>
+      </c>
+      <c r="F70" s="1">
+        <v>10</v>
+      </c>
+      <c r="G70" s="6">
+        <v>43925</v>
+      </c>
+      <c r="H70" s="6">
+        <v>43926</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B71" s="1">
+        <v>11</v>
+      </c>
+      <c r="C71" s="3">
+        <v>10021</v>
+      </c>
+      <c r="F71" s="1">
+        <v>11</v>
+      </c>
+      <c r="G71" s="6">
+        <v>43878</v>
+      </c>
+      <c r="H71" s="6">
+        <v>43880</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B72" s="1">
+        <v>12</v>
+      </c>
+      <c r="C72" s="3">
+        <v>10021</v>
+      </c>
+      <c r="F72" s="1">
+        <v>12</v>
+      </c>
+      <c r="G72" s="6">
+        <v>43913</v>
+      </c>
+      <c r="H72" s="6">
+        <v>43918</v>
+      </c>
+      <c r="I72" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>